<commit_message>
ms R1 first commit
</commit_message>
<xml_diff>
--- a/manuscript/SuppTables_S1234.xlsx
+++ b/manuscript/SuppTables_S1234.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yassato/Documents/GitHub/AraAphidGWAS/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116F5398-5A37-834A-8941-F9B4B0AE1679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92457697-1605-F74A-9A76-A95DBA643B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38060" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="4" xr2:uid="{1DD2B6DA-FD47-A647-9431-CDBFD348A53C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="4" xr2:uid="{1DD2B6DA-FD47-A647-9431-CDBFD348A53C}"/>
   </bookViews>
   <sheets>
     <sheet name="TableS1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="100">
   <si>
     <t>gwasID</t>
   </si>
@@ -372,6 +372,15 @@
   <si>
     <t>Without offset</t>
   </si>
+  <si>
+    <t>F-statistic and its p-value are shown for the effects of the mutant or wild type on the number of aphids, where df1 = 1 and df2 = 9 for the F-test.</t>
+  </si>
+  <si>
+    <t>The results at 7, 10, and 14 days after the release of aphids are shown without any offset terms, with initial plant size offset, or with flowering time offset.</t>
+  </si>
+  <si>
+    <t>Table SX. Nested Poisson GLMM comparing the number of aphids between the mutant and wild type plants.</t>
+  </si>
 </sst>
 </file>
 
@@ -568,19 +577,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -23606,14 +23615,14 @@
       <c r="A3" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="25" t="s">
         <v>74</v>
       </c>
@@ -23757,126 +23766,141 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E0FD47-6708-3649-80ED-91B76C67BDA8}">
-  <dimension ref="A2:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="30"/>
-    </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33" t="s">
+      <c r="G4" s="33"/>
+    </row>
+    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C5" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D5" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E5" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F5" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G5" s="31" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="6" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>19.3</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>1.7373849999999999E-3</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>6.9116999999999997</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>2.7402920000000001E-2</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>40.78</v>
       </c>
-      <c r="G4">
+      <c r="G6">
         <v>1.2736679999999999E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>56.957000000000001</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C7" s="27">
         <v>3.5155479999999998E-5</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <v>26.997</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>5.6719229999999999E-4</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>102.54</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G7" s="27">
         <v>3.2229760000000001E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B8" s="2">
         <v>131.27000000000001</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C8" s="29">
         <v>1.14101E-6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D8" s="2">
         <v>56.287999999999997</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E8" s="29">
         <v>3.6829019999999997E-5</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F8" s="2">
         <v>248.07</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G8" s="29">
         <v>7.378711E-8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ms R1 2nd commit
</commit_message>
<xml_diff>
--- a/manuscript/SuppTables_S1234.xlsx
+++ b/manuscript/SuppTables_S1234.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yassato/Documents/GitHub/AraAphidGWAS/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92457697-1605-F74A-9A76-A95DBA643B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747ECA02-38D9-FC44-8444-944831CE0191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="4" xr2:uid="{1DD2B6DA-FD47-A647-9431-CDBFD348A53C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="TableS2" sheetId="2" r:id="rId2"/>
     <sheet name="TableS3" sheetId="3" r:id="rId3"/>
     <sheet name="TableS4" sheetId="4" r:id="rId4"/>
-    <sheet name="TableSX" sheetId="5" r:id="rId5"/>
+    <sheet name="TableS5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -379,7 +379,7 @@
     <t>The results at 7, 10, and 14 days after the release of aphids are shown without any offset terms, with initial plant size offset, or with flowering time offset.</t>
   </si>
   <si>
-    <t>Table SX. Nested Poisson GLMM comparing the number of aphids between the mutant and wild type plants.</t>
+    <t>Table S5. Analysis of deviance for GLMMs comparing the number of aphids between the mutant and wild type plants.</t>
   </si>
 </sst>
 </file>
@@ -23769,7 +23769,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>